<commit_message>
expanded pop dy model, contamination model, entanglement model
</commit_message>
<xml_diff>
--- a/tables/FigSX_dungenss_crab_timeline.xlsx
+++ b/tables/FigSX_dungenss_crab_timeline.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/dungeness/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92379305-8251-D74F-8494-C76790F8E60A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7F2299-B26E-D149-9F59-DFD6D72A1F50}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10840" yWindow="4520" windowWidth="40620" windowHeight="21180" xr2:uid="{B774C1BA-0B64-334B-992A-B41393F1F4E3}"/>
+    <workbookView xWindow="9220" yWindow="2260" windowWidth="40620" windowHeight="21180" xr2:uid="{B774C1BA-0B64-334B-992A-B41393F1F4E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -273,86 +274,86 @@
   </cellStyleXfs>
   <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -679,7 +680,7 @@
   <dimension ref="A2:AA16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -697,391 +698,391 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:27" ht="68" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="26"/>
+      <c r="D2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4" t="s">
+      <c r="E2" s="26"/>
+      <c r="F2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4" t="s">
+      <c r="G2" s="26"/>
+      <c r="H2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4" t="s">
+      <c r="I2" s="26"/>
+      <c r="J2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4" t="s">
+      <c r="K2" s="26"/>
+      <c r="L2" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4" t="s">
+      <c r="M2" s="26"/>
+      <c r="N2" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4" t="s">
+      <c r="O2" s="26"/>
+      <c r="P2" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4" t="s">
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="S2" s="22"/>
-      <c r="T2" s="4" t="s">
+      <c r="S2" s="27"/>
+      <c r="T2" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4" t="s">
+      <c r="U2" s="26"/>
+      <c r="V2" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4" t="s">
+      <c r="W2" s="26"/>
+      <c r="X2" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="18"/>
-      <c r="AA2" s="18"/>
+      <c r="Y2" s="26"/>
+      <c r="Z2" s="14"/>
+      <c r="AA2" s="14"/>
     </row>
     <row r="3" spans="1:27" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="23" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="16" t="s">
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="S3" s="24"/>
-      <c r="T3" s="17"/>
-      <c r="U3" s="17"/>
-      <c r="V3" s="17"/>
-      <c r="W3" s="11"/>
-      <c r="X3" s="16" t="s">
+      <c r="S3" s="21"/>
+      <c r="T3" s="13"/>
+      <c r="U3" s="13"/>
+      <c r="V3" s="13"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="Y3" s="16"/>
+      <c r="Y3" s="20"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="10" t="s">
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="19"/>
-      <c r="T4" s="11"/>
-      <c r="U4" s="11"/>
-      <c r="V4" s="11"/>
-      <c r="W4" s="11"/>
-      <c r="X4" s="11"/>
-      <c r="Y4" s="11"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="20"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="8"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="19"/>
-      <c r="T6" s="12"/>
-      <c r="U6" s="12"/>
-      <c r="V6" s="12"/>
-      <c r="W6" s="12"/>
-      <c r="X6" s="2"/>
-      <c r="Y6" s="2"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="19"/>
-      <c r="T7" s="11"/>
-      <c r="U7" s="11"/>
-      <c r="V7" s="11"/>
-      <c r="W7" s="7"/>
-      <c r="X7" s="7"/>
-      <c r="Y7" s="7"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="20"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
-      <c r="V8" s="8"/>
-      <c r="W8" s="8"/>
-      <c r="X8" s="8"/>
-      <c r="Y8" s="8"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="19"/>
-      <c r="T9" s="11"/>
-      <c r="U9" s="11"/>
-      <c r="V9" s="11"/>
-      <c r="W9" s="11"/>
-      <c r="X9" s="15"/>
-      <c r="Y9" s="15"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="12"/>
+      <c r="Y9" s="12"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="21"/>
-      <c r="T10" s="9"/>
-      <c r="U10" s="9"/>
-      <c r="V10" s="9"/>
-      <c r="W10" s="9"/>
-      <c r="X10" s="11"/>
-      <c r="Y10" s="11"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="17"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
+      <c r="V10" s="7"/>
+      <c r="W10" s="7"/>
+      <c r="X10" s="8"/>
+      <c r="Y10" s="8"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
-      <c r="S11" s="20"/>
-      <c r="T11" s="3"/>
-      <c r="U11" s="3"/>
-      <c r="V11" s="3"/>
-      <c r="W11" s="3"/>
-      <c r="X11" s="3"/>
-      <c r="Y11" s="3"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="16"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="11"/>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="11"/>
-      <c r="S12" s="19"/>
-      <c r="T12" s="25" t="s">
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="U12" s="26"/>
-      <c r="V12" s="26"/>
-      <c r="W12" s="11"/>
-      <c r="X12" s="11"/>
-      <c r="Y12" s="11"/>
+      <c r="U12" s="23"/>
+      <c r="V12" s="23"/>
+      <c r="W12" s="8"/>
+      <c r="X12" s="8"/>
+      <c r="Y12" s="8"/>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="1" t="s">
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="1" t="s">
+      <c r="E13" s="19"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="1" t="s">
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="O13" s="1"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="11"/>
-      <c r="S13" s="19"/>
-      <c r="T13" s="27" t="s">
+      <c r="O13" s="19"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="U13" s="1"/>
-      <c r="V13" s="1"/>
-      <c r="W13" s="1"/>
-      <c r="X13" s="11"/>
-      <c r="Y13" s="11"/>
+      <c r="U13" s="19"/>
+      <c r="V13" s="19"/>
+      <c r="W13" s="19"/>
+      <c r="X13" s="8"/>
+      <c r="Y13" s="8"/>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1090,13 +1091,11 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="T13:W13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="T12:V12"/>
-    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
     <mergeCell ref="X3:Y3"/>
     <mergeCell ref="H4:K4"/>
     <mergeCell ref="F3:M3"/>
@@ -1106,12 +1105,14 @@
     <mergeCell ref="T2:U2"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
     <mergeCell ref="L2:M2"/>
+    <mergeCell ref="T13:W13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="T12:V12"/>
+    <mergeCell ref="B4:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup fitToWidth="4" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>